<commit_message>
4 clusters for relays
</commit_message>
<xml_diff>
--- a/Projects/zstack/HomeAutomation/cc2530/code/_docs/gpio_used.xlsx
+++ b/Projects/zstack/HomeAutomation/cc2530/code/_docs/gpio_used.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
     <t>P0_0</t>
   </si>
@@ -137,9 +137,6 @@
     <t>BTN #1</t>
   </si>
   <si>
-    <t>OLED CS</t>
-  </si>
-  <si>
     <t>LED #2</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
   </si>
   <si>
     <t>Flash DC</t>
-  </si>
-  <si>
-    <t>can be grounded (P0_2=0)</t>
   </si>
   <si>
     <t>DHT11</t>
@@ -587,7 +581,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -647,21 +643,17 @@
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
@@ -684,7 +676,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>25</v>
@@ -729,7 +721,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>25</v>
@@ -744,7 +736,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>26</v>
@@ -756,7 +748,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>23</v>
@@ -789,7 +781,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>25</v>
@@ -801,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>24</v>
@@ -819,7 +811,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>25</v>
@@ -861,7 +853,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>23</v>
@@ -877,7 +869,7 @@
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>25</v>
@@ -892,7 +884,7 @@
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
4 cluster for relay => z2m
</commit_message>
<xml_diff>
--- a/Projects/zstack/HomeAutomation/cc2530/code/_docs/gpio_used.xlsx
+++ b/Projects/zstack/HomeAutomation/cc2530/code/_docs/gpio_used.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>P0_0</t>
   </si>
@@ -146,9 +146,6 @@
     <t>BTN #2</t>
   </si>
   <si>
-    <t>LED Green</t>
-  </si>
-  <si>
     <t>Relay</t>
   </si>
   <si>
@@ -165,6 +162,12 @@
   </si>
   <si>
     <t>DHT11</t>
+  </si>
+  <si>
+    <t>OLED CS</t>
+  </si>
+  <si>
+    <t>LED Green?</t>
   </si>
 </sst>
 </file>
@@ -579,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F21"/>
+  <dimension ref="B2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +598,7 @@
     <col min="6" max="6" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
@@ -612,7 +615,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
@@ -627,7 +630,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
@@ -642,20 +645,22 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
@@ -668,22 +673,23 @@
       </c>
       <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="11"/>
+      <c r="E7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>5</v>
       </c>
@@ -698,7 +704,7 @@
       </c>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>6</v>
       </c>
@@ -713,7 +719,7 @@
       </c>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>7</v>
       </c>
@@ -721,14 +727,14 @@
         <v>19</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>8</v>
       </c>
@@ -736,14 +742,14 @@
         <v>34</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
         <v>9</v>
       </c>
@@ -758,7 +764,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>10</v>
       </c>
@@ -773,7 +779,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
         <v>11</v>
       </c>
@@ -781,14 +787,14 @@
         <v>21</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
         <v>12</v>
       </c>
@@ -803,7 +809,7 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>13</v>
       </c>
@@ -811,7 +817,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>25</v>
@@ -869,7 +875,7 @@
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>25</v>
@@ -884,7 +890,7 @@
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
DHT11 jn any port
</commit_message>
<xml_diff>
--- a/Projects/zstack/HomeAutomation/cc2530/code/_docs/gpio_used.xlsx
+++ b/Projects/zstack/HomeAutomation/cc2530/code/_docs/gpio_used.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>P0_0</t>
   </si>
@@ -161,13 +161,25 @@
     <t>Flash DC</t>
   </si>
   <si>
-    <t>DHT11</t>
-  </si>
-  <si>
     <t>OLED CS</t>
   </si>
   <si>
     <t>LED Green?</t>
+  </si>
+  <si>
+    <t>Relay #1</t>
+  </si>
+  <si>
+    <t>DHT11, Relay #4</t>
+  </si>
+  <si>
+    <t>Relay #2</t>
+  </si>
+  <si>
+    <t>Relay #3</t>
+  </si>
+  <si>
+    <t>DHT11?</t>
   </si>
 </sst>
 </file>
@@ -585,7 +597,7 @@
   <dimension ref="B2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +605,7 @@
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" customWidth="1"/>
   </cols>
@@ -650,7 +662,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>23</v>
@@ -680,13 +692,15 @@
       <c r="C7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="E7" s="10" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -697,7 +711,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>25</v>
@@ -712,7 +726,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>25</v>
@@ -727,7 +741,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>25</v>
@@ -832,7 +846,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>25</v>

</xml_diff>